<commit_message>
Added upload api endpoint info
</commit_message>
<xml_diff>
--- a/Backend/Info/Api Paths.xlsx
+++ b/Backend/Info/Api Paths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>path</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Response</t>
-  </si>
-  <si>
-    <t>Email,Password</t>
   </si>
   <si>
     <t>Token with status</t>
@@ -83,6 +80,34 @@
   </si>
   <si>
     <t>Info on created user</t>
+  </si>
+  <si>
+    <t>Email
+Password</t>
+  </si>
+  <si>
+    <t>add single or multiple files to the server</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The path to the file </t>
+  </si>
+  <si>
+    <t>file(single/multiple)</t>
+  </si>
+  <si>
+    <t>/upload/</t>
+  </si>
+  <si>
+    <t>/upload/file</t>
+  </si>
+  <si>
+    <t>get a list of all the files</t>
+  </si>
+  <si>
+    <t>All the files in the uploads folder</t>
   </si>
 </sst>
 </file>
@@ -125,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -133,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,8 +475,8 @@
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
@@ -462,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -482,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -496,10 +524,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -507,36 +535,73 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mail api routes
</commit_message>
<xml_diff>
--- a/Backend/Info/Api Paths.xlsx
+++ b/Backend/Info/Api Paths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>path</t>
   </si>
@@ -108,6 +108,29 @@
   </si>
   <si>
     <t>All the files in the uploads folder</t>
+  </si>
+  <si>
+    <t>/mail/send</t>
+  </si>
+  <si>
+    <t>/mail/send-multiple</t>
+  </si>
+  <si>
+    <t>send mail to a single user</t>
+  </si>
+  <si>
+    <t>send mail to multiple users</t>
+  </si>
+  <si>
+    <t>Email
+Body</t>
+  </si>
+  <si>
+    <t>EmailAddresses
+Body</t>
+  </si>
+  <si>
+    <t>status and message</t>
   </si>
 </sst>
 </file>
@@ -463,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +625,46 @@
       </c>
       <c r="F7" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>